<commit_message>
Update 30 November 2023 - Change return Class Validation request
</commit_message>
<xml_diff>
--- a/public/template_import/TEMPLATE_IMPORT_POTONGAN.xlsx
+++ b/public/template_import/TEMPLATE_IMPORT_POTONGAN.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">KD_PGW</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">ABC</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
+    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">2023-11</t>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">DEF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
   </si>
 </sst>
 </file>
@@ -199,11 +196,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.80078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="27.80859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.5"/>
@@ -261,7 +258,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Update 03 February  2024 - Import validation
</commit_message>
<xml_diff>
--- a/public/template_import/TEMPLATE_IMPORT_POTONGAN.xlsx
+++ b/public/template_import/TEMPLATE_IMPORT_POTONGAN.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t xml:space="preserve">KD_PGW</t>
   </si>
@@ -35,6 +35,27 @@
   </si>
   <si>
     <t xml:space="preserve">PERIODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0324230001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0324230002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0324230003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0324230004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0324230005</t>
   </si>
 </sst>
 </file>
@@ -69,7 +90,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,12 +99,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFB2B2B2"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -98,6 +125,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -124,7 +158,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -141,16 +175,20 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -178,7 +216,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB2B2B2"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -211,7 +249,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -230,22 +268,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ31"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.8359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="27.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="27.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="27.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -267,34 +306,89 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
+      <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0"/>
-      <c r="C4" s="0"/>
-      <c r="D4" s="0"/>
-      <c r="E4" s="0"/>
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0"/>
-      <c r="C5" s="0"/>
-      <c r="D5" s="0"/>
-      <c r="E5" s="0"/>
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0"/>
-      <c r="C6" s="0"/>
-      <c r="D6" s="0"/>
-      <c r="E6" s="0"/>
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0"/>
@@ -440,12 +534,7 @@
       <c r="D30" s="0"/>
       <c r="E30" s="0"/>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0"/>
-      <c r="C31" s="0"/>
-      <c r="D31" s="0"/>
-      <c r="E31" s="0"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>